<commit_message>
PTW: AXI4 Redesigned, Test added
</commit_message>
<xml_diff>
--- a/docs/Fetch.xlsx
+++ b/docs/Fetch.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Armleo\Desktop\armleocpu\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A82D79C0-C57B-4A72-8B28-AA21B19D56D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8D3227C6-4F5A-499A-844C-5A50E5C92D13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="146" uniqueCount="60">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="170" uniqueCount="64">
   <si>
     <t>after_flush</t>
   </si>
@@ -206,12 +206,24 @@
   </si>
   <si>
     <t>pc_is_next_pc</t>
+  </si>
+  <si>
+    <t>INTERRUPT_PENDING</t>
+  </si>
+  <si>
+    <t>abort</t>
+  </si>
+  <si>
+    <t>abort because IRQ handling</t>
+  </si>
+  <si>
+    <t>not ready</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,24 +413,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
+    <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -729,7 +741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1284,11 +1296,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1297,11 +1309,11 @@
     <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.75" customWidth="1"/>
     <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1517,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -1529,13 +1541,125 @@
         <v>46</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>